<commit_message>
Some improvements in the dynamism of the project
</commit_message>
<xml_diff>
--- a/Dispatcher/Data/Config.xlsx
+++ b/Dispatcher/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omarf\Desktop\ITI\During Sessions\UIpath\Labs\Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074DF094-D75E-42A6-85B7-169C522242CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75762160-6B63-483A-994D-C42221D1D99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -186,6 +186,27 @@
   </si>
   <si>
     <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>WorkItemWIID</t>
+  </si>
+  <si>
+    <t>WI3</t>
+  </si>
+  <si>
+    <t>Which wiid you want to extract</t>
+  </si>
+  <si>
+    <t>WorkItemsPages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of pages in work items section </t>
+  </si>
+  <si>
+    <t>ProcessNames</t>
+  </si>
+  <si>
+    <t>excel;chrome</t>
   </si>
 </sst>
 </file>
@@ -565,7 +586,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -684,9 +705,36 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Some Improvements to the project organization
</commit_message>
<xml_diff>
--- a/Dispatcher/Data/Config.xlsx
+++ b/Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omarf\Desktop\ITI\During Sessions\UIpath\Labs\Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75762160-6B63-483A-994D-C42221D1D99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF68C63-7955-4B90-B69E-492D95E33126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -191,9 +191,6 @@
     <t>WorkItemWIID</t>
   </si>
   <si>
-    <t>WI3</t>
-  </si>
-  <si>
     <t>Which wiid you want to extract</t>
   </si>
   <si>
@@ -207,6 +204,18 @@
   </si>
   <si>
     <t>excel;chrome</t>
+  </si>
+  <si>
+    <t>WIStatus</t>
+  </si>
+  <si>
+    <t>WIType</t>
+  </si>
+  <si>
+    <t>MaxPages</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -585,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -707,34 +716,14 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2894,8 +2883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2942,9 +2931,45 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>